<commit_message>
add new table t_app_data_version_list
</commit_message>
<xml_diff>
--- a/cfg/schema/test_game_system.xlsx
+++ b/cfg/schema/test_game_system.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="560" windowWidth="31540" windowHeight="17660" tabRatio="943" firstSheet="5" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="943" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="2" r:id="rId1"/>
     <sheet name="T_APP_BASE" sheetId="1" r:id="rId2"/>
     <sheet name="T_APP_DATA" sheetId="16" r:id="rId3"/>
     <sheet name="T_APP_DATA_VERSION" sheetId="17" r:id="rId4"/>
-    <sheet name="T_APP_DATA_GROUP" sheetId="20" r:id="rId5"/>
-    <sheet name="T_APP_DATA_GROUP_DETAIL" sheetId="21" r:id="rId6"/>
-    <sheet name="T_APP_CLIENT" sheetId="14" r:id="rId7"/>
-    <sheet name="T_APP_SERVER" sheetId="11" r:id="rId8"/>
-    <sheet name="T_APP_PROPERTY" sheetId="7" r:id="rId9"/>
-    <sheet name="T_APP_REGISTER" sheetId="27" r:id="rId10"/>
-    <sheet name="T_APP_GLOBAL" sheetId="13" r:id="rId11"/>
-    <sheet name="T_SERVICE_DEPLOY" sheetId="6" r:id="rId12"/>
-    <sheet name="T_EVENT" sheetId="22" r:id="rId13"/>
-    <sheet name="T_EVENT_REWARD" sheetId="23" r:id="rId14"/>
-    <sheet name="T_EVENT_REWARD_DETAIL" sheetId="24" r:id="rId15"/>
-    <sheet name="T_EVENT_LOCALIZATION" sheetId="25" r:id="rId16"/>
-    <sheet name="T_MON_SERVICE" sheetId="28" r:id="rId17"/>
-    <sheet name="T_SERVICE_DEPLOYS" sheetId="29" r:id="rId18"/>
-    <sheet name="T_MSG_HOST" sheetId="30" r:id="rId19"/>
+    <sheet name="T_APP_DATA_VERSION_LIST" sheetId="31" r:id="rId5"/>
+    <sheet name="T_APP_DATA_GROUP" sheetId="20" r:id="rId6"/>
+    <sheet name="T_APP_DATA_GROUP_DETAIL" sheetId="21" r:id="rId7"/>
+    <sheet name="T_APP_CLIENT" sheetId="14" r:id="rId8"/>
+    <sheet name="T_APP_SERVER" sheetId="11" r:id="rId9"/>
+    <sheet name="T_APP_PROPERTY" sheetId="7" r:id="rId10"/>
+    <sheet name="T_APP_REGISTER" sheetId="27" r:id="rId11"/>
+    <sheet name="T_APP_GLOBAL" sheetId="13" r:id="rId12"/>
+    <sheet name="T_SERVICE_DEPLOY" sheetId="6" r:id="rId13"/>
+    <sheet name="T_EVENT" sheetId="22" r:id="rId14"/>
+    <sheet name="T_EVENT_REWARD" sheetId="23" r:id="rId15"/>
+    <sheet name="T_EVENT_REWARD_DETAIL" sheetId="24" r:id="rId16"/>
+    <sheet name="T_EVENT_LOCALIZATION" sheetId="25" r:id="rId17"/>
+    <sheet name="T_MON_SERVICE" sheetId="28" r:id="rId18"/>
+    <sheet name="T_SERVICE_DEPLOYS" sheetId="29" r:id="rId19"/>
+    <sheet name="T_MSG_HOST" sheetId="30" r:id="rId20"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="340">
   <si>
     <t>Name</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1362,6 +1363,24 @@
   </si>
   <si>
     <t>T_SERVICE_DEPLOYS</t>
+  </si>
+  <si>
+    <t>T_APP_DATA_VERSION_LIST</t>
+  </si>
+  <si>
+    <t>versionList</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>not</t>
   </si>
 </sst>
 </file>
@@ -1372,28 +1391,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1402,14 +1421,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1418,7 +1437,7 @@
       <u/>
       <sz val="9"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1426,13 +1445,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1440,7 +1459,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1483,10 +1502,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1534,14 +1556,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
-    <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준 5" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1844,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -1948,62 +1973,60 @@
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>124</v>
+        <v>111</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>335</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>172</v>
+        <v>334</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>124</v>
+        <v>172</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="13.5" customHeight="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="11.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>109</v>
+        <v>126</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="13.5" customHeight="1">
@@ -2011,17 +2034,19 @@
         <v>111</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13.5" customHeight="1">
@@ -2029,80 +2054,82 @@
         <v>111</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>215</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="13.5" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>238</v>
+        <v>111</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>240</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>214</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="12">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="13.5" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>99</v>
+        <v>240</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>94</v>
+        <v>259</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="13.5" customHeight="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="12">
       <c r="A12" s="4" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>226</v>
+        <v>94</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="13.5" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -2115,14 +2142,12 @@
         <v>161</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -2133,13 +2158,13 @@
         <v>161</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -2147,17 +2172,17 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>261</v>
+      <c r="A16" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>165</v>
+        <v>234</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -2166,15 +2191,17 @@
     </row>
     <row r="17" spans="1:8" ht="13.5" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="D17" s="4"/>
+        <v>261</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -2182,13 +2209,13 @@
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>330</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>333</v>
+        <v>278</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2198,13 +2225,13 @@
     </row>
     <row r="19" spans="1:8" ht="13.5" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>330</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2212,26 +2239,42 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
+    <row r="20" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C3" location="T_APP_DATA!A1" display="T_APP_DATA"/>
     <hyperlink ref="C4" location="T_APP_DATA_VERSION!A1" display="T_APP_DATA_VERSION"/>
-    <hyperlink ref="C5" location="T_APP_DATA_GROUP!A1" display="T_APP_DATA_GROUP"/>
-    <hyperlink ref="C6" location="T_APP_DATA_GROUP_DETAIL!A1" display="T_APP_DATA_GROUP_DETAIL"/>
-    <hyperlink ref="C7" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
-    <hyperlink ref="C13" location="T_EVENT!A1" display="T_EVENT_MAIN"/>
-    <hyperlink ref="C14" location="T_EVENT_REWARD!A1" display="T_EVENT_REWARD"/>
-    <hyperlink ref="C15" location="T_EVENT_REWARDS_DETAIL!A1" display="T_EVENT_REWARDS_DETAIL"/>
-    <hyperlink ref="C16" location="T_EVENT_LOCALIZATION!A1" display="T_EVENT_LOCALIZATION"/>
+    <hyperlink ref="C6" location="T_APP_DATA_GROUP!A1" display="T_APP_DATA_GROUP"/>
+    <hyperlink ref="C7" location="T_APP_DATA_GROUP_DETAIL!A1" display="T_APP_DATA_GROUP_DETAIL"/>
+    <hyperlink ref="C8" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
+    <hyperlink ref="C14" location="T_EVENT!A1" display="T_EVENT_MAIN"/>
+    <hyperlink ref="C15" location="T_EVENT_REWARD!A1" display="T_EVENT_REWARD"/>
+    <hyperlink ref="C16" location="T_EVENT_REWARDS_DETAIL!A1" display="T_EVENT_REWARDS_DETAIL"/>
+    <hyperlink ref="C17" location="T_EVENT_LOCALIZATION!A1" display="T_EVENT_LOCALIZATION"/>
     <hyperlink ref="C2" location="T_APP_BASE!A1" display="T_APP_BASE"/>
-    <hyperlink ref="C12" location="T_SERVICE_DEPLOY!A1" display="T_SERVICE_DEPLOY"/>
-    <hyperlink ref="C11" location="T_APP_GLOBAL!A1" display="T_APP_GLOBAL"/>
-    <hyperlink ref="C8" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
-    <hyperlink ref="C9" location="T_APP_PROPERTY!A1" display="T_APP_PROPERTY"/>
-    <hyperlink ref="C17" location="T_MON_SERVICE!A1" display="T_MON_SERVICE"/>
-    <hyperlink ref="C18" location="T_SERVICE_DEPLOYS!A1" display="T_SERVICE_DEPLOYS"/>
-    <hyperlink ref="C19" location="T_MSG_HOST!A1" display="T_MSG_HOST"/>
+    <hyperlink ref="C13" location="T_SERVICE_DEPLOY!A1" display="T_SERVICE_DEPLOY"/>
+    <hyperlink ref="C12" location="T_APP_GLOBAL!A1" display="T_APP_GLOBAL"/>
+    <hyperlink ref="C9" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
+    <hyperlink ref="C10" location="T_APP_PROPERTY!A1" display="T_APP_PROPERTY"/>
+    <hyperlink ref="C18" location="T_MON_SERVICE!A1" display="T_MON_SERVICE"/>
+    <hyperlink ref="C19" location="T_SERVICE_DEPLOYS!A1" display="T_SERVICE_DEPLOYS"/>
+    <hyperlink ref="C20" location="T_MSG_HOST!A1" display="T_MSG_HOST"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2244,6 +2287,118 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="12">
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2393,7 +2548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2501,7 +2656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -2631,7 +2786,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2640,7 +2794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -3040,7 +3194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
@@ -3400,7 +3554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -3559,7 +3713,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3568,7 +3721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -3731,7 +3884,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3740,7 +3892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -3949,194 +4101,6 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="6" max="6" width="33.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="D2" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4150,162 +4114,172 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="11" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>49</v>
+        <v>287</v>
       </c>
       <c r="D2" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>325</v>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="16" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="17" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>311</v>
+        <v>50</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="17" t="s">
-        <v>326</v>
+      <c r="F4" s="12" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>312</v>
+        <v>62</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>313</v>
+        <v>26</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>298</v>
+        <v>49</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11" t="s">
-        <v>314</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="16" t="s">
-        <v>315</v>
+        <v>68</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>316</v>
+        <v>88</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>317</v>
+        <v>49</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>318</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="16" t="s">
-        <v>319</v>
+        <v>71</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>320</v>
+        <v>88</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>297</v>
+        <v>49</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11" t="s">
-        <v>321</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="16" t="s">
-        <v>322</v>
+        <v>66</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>297</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11" t="s">
-        <v>324</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>296</v>
+      </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -4421,7 +4395,182 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4560,7 +4709,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -4689,6 +4838,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4698,6 +4848,80 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -4807,7 +5031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -4934,7 +5158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5034,7 +5258,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5043,7 +5266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -5218,119 +5441,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="12">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="12">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="12">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12">
-      <c r="A4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12">
-      <c r="A5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
check excel sheet name
</commit_message>
<xml_diff>
--- a/cfg/schema/test_game_system.xlsx
+++ b/cfg/schema/test_game_system.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26423"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="943" activeTab="4"/>
+    <workbookView xWindow="7860" yWindow="2400" windowWidth="25600" windowHeight="16060" tabRatio="943" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="342">
   <si>
     <t>Name</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1381,6 +1381,14 @@
   </si>
   <si>
     <t>not</t>
+  </si>
+  <si>
+    <t>excel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>not</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1391,28 +1399,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1421,14 +1429,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1437,7 +1445,7 @@
       <u/>
       <sz val="9"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1445,13 +1453,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1459,7 +1467,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1502,10 +1510,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1556,17 +1568,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="15">
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준 5" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4408,7 +4424,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4583,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -4658,7 +4674,9 @@
       <c r="C4" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>85</v>
       </c>
@@ -4696,6 +4714,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4706,10 +4725,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -4775,63 +4794,80 @@
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>114</v>
+        <v>340</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>341</v>
       </c>
       <c r="D4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4851,7 +4887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4911,6 +4947,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -5033,10 +5070,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -5119,31 +5156,48 @@
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>177</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new table t_app_data_file_version
</commit_message>
<xml_diff>
--- a/cfg/schema/test_game_system.xlsx
+++ b/cfg/schema/test_game_system.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="2400" windowWidth="25600" windowHeight="16060" tabRatio="943" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="943" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="2" r:id="rId1"/>
     <sheet name="T_APP_BASE" sheetId="1" r:id="rId2"/>
     <sheet name="T_APP_DATA" sheetId="16" r:id="rId3"/>
-    <sheet name="T_APP_DATA_VERSION" sheetId="17" r:id="rId4"/>
-    <sheet name="T_APP_DATA_VERSION_LIST" sheetId="31" r:id="rId5"/>
-    <sheet name="T_APP_DATA_GROUP" sheetId="20" r:id="rId6"/>
-    <sheet name="T_APP_DATA_GROUP_DETAIL" sheetId="21" r:id="rId7"/>
-    <sheet name="T_APP_CLIENT" sheetId="14" r:id="rId8"/>
-    <sheet name="T_APP_SERVER" sheetId="11" r:id="rId9"/>
-    <sheet name="T_APP_PROPERTY" sheetId="7" r:id="rId10"/>
-    <sheet name="T_APP_REGISTER" sheetId="27" r:id="rId11"/>
-    <sheet name="T_APP_GLOBAL" sheetId="13" r:id="rId12"/>
-    <sheet name="T_SERVICE_DEPLOY" sheetId="6" r:id="rId13"/>
-    <sheet name="T_EVENT" sheetId="22" r:id="rId14"/>
-    <sheet name="T_EVENT_REWARD" sheetId="23" r:id="rId15"/>
-    <sheet name="T_EVENT_REWARD_DETAIL" sheetId="24" r:id="rId16"/>
-    <sheet name="T_EVENT_LOCALIZATION" sheetId="25" r:id="rId17"/>
-    <sheet name="T_MON_SERVICE" sheetId="28" r:id="rId18"/>
-    <sheet name="T_SERVICE_DEPLOYS" sheetId="29" r:id="rId19"/>
-    <sheet name="T_MSG_HOST" sheetId="30" r:id="rId20"/>
+    <sheet name="T_APP_DATA_FILE_VERSION" sheetId="32" r:id="rId4"/>
+    <sheet name="T_APP_DATA_VERSION" sheetId="17" r:id="rId5"/>
+    <sheet name="T_APP_DATA_VERSION_LIST" sheetId="31" r:id="rId6"/>
+    <sheet name="T_APP_DATA_GROUP" sheetId="20" r:id="rId7"/>
+    <sheet name="T_APP_DATA_GROUP_DETAIL" sheetId="21" r:id="rId8"/>
+    <sheet name="T_APP_CLIENT" sheetId="14" r:id="rId9"/>
+    <sheet name="T_APP_SERVER" sheetId="11" r:id="rId10"/>
+    <sheet name="T_APP_PROPERTY" sheetId="7" r:id="rId11"/>
+    <sheet name="T_APP_REGISTER" sheetId="27" r:id="rId12"/>
+    <sheet name="T_APP_GLOBAL" sheetId="13" r:id="rId13"/>
+    <sheet name="T_SERVICE_DEPLOY" sheetId="6" r:id="rId14"/>
+    <sheet name="T_EVENT" sheetId="22" r:id="rId15"/>
+    <sheet name="T_EVENT_REWARD" sheetId="23" r:id="rId16"/>
+    <sheet name="T_EVENT_REWARD_DETAIL" sheetId="24" r:id="rId17"/>
+    <sheet name="T_EVENT_LOCALIZATION" sheetId="25" r:id="rId18"/>
+    <sheet name="T_MON_SERVICE" sheetId="28" r:id="rId19"/>
+    <sheet name="T_SERVICE_DEPLOYS" sheetId="29" r:id="rId20"/>
+    <sheet name="T_MSG_HOST" sheetId="30" r:id="rId21"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="344">
   <si>
     <t>Name</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1389,6 +1390,12 @@
   <si>
     <t>not</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>T_APP_DATA_FILE_VERSION</t>
   </si>
 </sst>
 </file>
@@ -1399,28 +1406,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1429,14 +1436,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1445,7 +1452,7 @@
       <u/>
       <sz val="9"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1453,13 +1460,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1467,7 +1474,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1510,10 +1517,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1568,21 +1578,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
-    <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+  <cellStyles count="18">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준 5" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1885,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -1971,98 +1984,94 @@
       <c r="A4" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>106</v>
+      <c r="B4" s="3" t="s">
+        <v>342</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>110</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4" t="s">
-        <v>128</v>
-      </c>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>335</v>
+      <c r="B5" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>334</v>
+        <v>107</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>124</v>
+        <v>111</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>335</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>172</v>
+        <v>334</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="11.25" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>124</v>
+        <v>172</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="13.5" customHeight="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="11.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>109</v>
+        <v>126</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13.5" customHeight="1">
@@ -2070,17 +2079,19 @@
         <v>111</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13.5" customHeight="1">
@@ -2088,80 +2099,82 @@
         <v>111</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>215</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="13.5" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>238</v>
+        <v>111</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>240</v>
+        <v>33</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>214</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="12">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="13.5" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>99</v>
+        <v>240</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>94</v>
+        <v>259</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="13.5" customHeight="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="12">
       <c r="A13" s="4" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>226</v>
+        <v>94</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -2174,14 +2187,12 @@
         <v>161</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -2192,13 +2203,13 @@
         <v>161</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -2206,17 +2217,17 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>261</v>
+      <c r="A17" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>165</v>
+        <v>234</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -2225,15 +2236,17 @@
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="D18" s="4"/>
+        <v>261</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -2241,13 +2254,13 @@
     </row>
     <row r="19" spans="1:8" ht="13.5" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>330</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>333</v>
+        <v>278</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2257,13 +2270,13 @@
     </row>
     <row r="20" spans="1:8" ht="13.5" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>330</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2271,26 +2284,42 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
+    <row r="21" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C3" location="T_APP_DATA!A1" display="T_APP_DATA"/>
-    <hyperlink ref="C4" location="T_APP_DATA_VERSION!A1" display="T_APP_DATA_VERSION"/>
-    <hyperlink ref="C6" location="T_APP_DATA_GROUP!A1" display="T_APP_DATA_GROUP"/>
-    <hyperlink ref="C7" location="T_APP_DATA_GROUP_DETAIL!A1" display="T_APP_DATA_GROUP_DETAIL"/>
-    <hyperlink ref="C8" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
-    <hyperlink ref="C14" location="T_EVENT!A1" display="T_EVENT_MAIN"/>
-    <hyperlink ref="C15" location="T_EVENT_REWARD!A1" display="T_EVENT_REWARD"/>
-    <hyperlink ref="C16" location="T_EVENT_REWARDS_DETAIL!A1" display="T_EVENT_REWARDS_DETAIL"/>
-    <hyperlink ref="C17" location="T_EVENT_LOCALIZATION!A1" display="T_EVENT_LOCALIZATION"/>
+    <hyperlink ref="C5" location="T_APP_DATA_VERSION!A1" display="T_APP_DATA_VERSION"/>
+    <hyperlink ref="C7" location="T_APP_DATA_GROUP!A1" display="T_APP_DATA_GROUP"/>
+    <hyperlink ref="C8" location="T_APP_DATA_GROUP_DETAIL!A1" display="T_APP_DATA_GROUP_DETAIL"/>
+    <hyperlink ref="C9" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
+    <hyperlink ref="C15" location="T_EVENT!A1" display="T_EVENT_MAIN"/>
+    <hyperlink ref="C16" location="T_EVENT_REWARD!A1" display="T_EVENT_REWARD"/>
+    <hyperlink ref="C17" location="T_EVENT_REWARDS_DETAIL!A1" display="T_EVENT_REWARDS_DETAIL"/>
+    <hyperlink ref="C18" location="T_EVENT_LOCALIZATION!A1" display="T_EVENT_LOCALIZATION"/>
     <hyperlink ref="C2" location="T_APP_BASE!A1" display="T_APP_BASE"/>
-    <hyperlink ref="C13" location="T_SERVICE_DEPLOY!A1" display="T_SERVICE_DEPLOY"/>
-    <hyperlink ref="C12" location="T_APP_GLOBAL!A1" display="T_APP_GLOBAL"/>
-    <hyperlink ref="C9" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
-    <hyperlink ref="C10" location="T_APP_PROPERTY!A1" display="T_APP_PROPERTY"/>
-    <hyperlink ref="C18" location="T_MON_SERVICE!A1" display="T_MON_SERVICE"/>
-    <hyperlink ref="C19" location="T_SERVICE_DEPLOYS!A1" display="T_SERVICE_DEPLOYS"/>
-    <hyperlink ref="C20" location="T_MSG_HOST!A1" display="T_MSG_HOST"/>
+    <hyperlink ref="C14" location="T_SERVICE_DEPLOY!A1" display="T_SERVICE_DEPLOY"/>
+    <hyperlink ref="C13" location="T_APP_GLOBAL!A1" display="T_APP_GLOBAL"/>
+    <hyperlink ref="C10" location="T_APP_CLIENT!A1" display="T_APP_CLIENT"/>
+    <hyperlink ref="C11" location="T_APP_PROPERTY!A1" display="T_APP_PROPERTY"/>
+    <hyperlink ref="C19" location="T_MON_SERVICE!A1" display="T_MON_SERVICE"/>
+    <hyperlink ref="C20" location="T_SERVICE_DEPLOYS!A1" display="T_SERVICE_DEPLOYS"/>
+    <hyperlink ref="C21" location="T_MSG_HOST!A1" display="T_MSG_HOST"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2303,6 +2332,189 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="12">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="12">
+      <c r="A3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="7" customFormat="1" ht="12">
+      <c r="A5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="7" customFormat="1" ht="12">
+      <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="7" customFormat="1" ht="12">
+      <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="7" customFormat="1" ht="12">
+      <c r="A8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12">
+      <c r="A9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="7" customFormat="1" ht="12">
+      <c r="A10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2414,7 +2626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2564,7 +2776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2672,7 +2884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -2810,7 +3022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -3210,7 +3422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
@@ -3570,7 +3782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -3737,7 +3949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -3908,7 +4120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -4116,192 +4328,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="6" max="6" width="33.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="D2" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4424,6 +4450,192 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="33.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -4599,7 +4811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -4714,7 +4926,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4725,10 +4936,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -4794,6 +5005,132 @@
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>340</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -4883,7 +5220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -4949,7 +5286,6 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4958,7 +5294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5068,7 +5404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -5212,7 +5548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5318,187 +5654,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="12">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="12">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" ht="12">
-      <c r="A3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="7" customFormat="1" ht="12">
-      <c r="A5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="7" customFormat="1" ht="12">
-      <c r="A6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="7" customFormat="1" ht="12">
-      <c r="A7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="7" customFormat="1" ht="12">
-      <c r="A8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12">
-      <c r="A9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="7" customFormat="1" ht="12">
-      <c r="A10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add new book file versiion
</commit_message>
<xml_diff>
--- a/cfg/schema/test_game_system.xlsx
+++ b/cfg/schema/test_game_system.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="943" activeTab="3"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="943"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="2" r:id="rId1"/>
@@ -1900,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -1987,7 +1987,7 @@
       <c r="B4" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="18" t="s">
         <v>343</v>
       </c>
       <c r="D4" s="4"/>
@@ -2320,9 +2320,9 @@
     <hyperlink ref="C19" location="T_MON_SERVICE!A1" display="T_MON_SERVICE"/>
     <hyperlink ref="C20" location="T_SERVICE_DEPLOYS!A1" display="T_SERVICE_DEPLOYS"/>
     <hyperlink ref="C21" location="T_MSG_HOST!A1" display="T_MSG_HOST"/>
+    <hyperlink ref="C4" location="T_APP_DATA_FILE_VERSION!A1" display="T_APP_DATA_FILE_VERSION"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4938,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -5211,7 +5211,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>